<commit_message>
Update for review 1 - Contribution Sheet
</commit_message>
<xml_diff>
--- a/Group 3 - Contribution Sheet.xlsx
+++ b/Group 3 - Contribution Sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2AA6D4A-6561-4600-9DC7-66DD8ADEC8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4935FC32-32B0-4EB3-A45B-5B469123A8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -478,7 +478,9 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -488,7 +490,9 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -498,7 +502,9 @@
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -508,7 +514,9 @@
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -518,7 +526,9 @@
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>20</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -530,7 +540,7 @@
       </c>
       <c r="B7" s="2">
         <f>SUM(B2:B6)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
         <f>SUM(C2:C6)</f>

</xml_diff>